<commit_message>
New randomizer based on probability
</commit_message>
<xml_diff>
--- a/WinnerWinnerChickenDinner/iattend output.xlsx
+++ b/WinnerWinnerChickenDinner/iattend output.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\source\repos\WinnerWinnerChickenDinner\WinnerWinnerChickenDinner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFB61A3E-B68F-464F-B94D-3EBC184569B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D9EF6F-24E4-484D-A965-78DD3327DFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7035" yWindow="3420" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ticket Information" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Number of tickets purchased</t>
   </si>
@@ -81,22 +81,7 @@
     <t>Edgar, Man</t>
   </si>
   <si>
-    <t>Asspol</t>
-  </si>
-  <si>
-    <t>Porral, Part</t>
-  </si>
-  <si>
-    <t>Bart Simpson</t>
-  </si>
-  <si>
-    <t>Yuelo, Buelo</t>
-  </si>
-  <si>
-    <t>Yami, Dami</t>
-  </si>
-  <si>
-    <t>Just A Man</t>
+    <t>BEST WINNER</t>
   </si>
 </sst>
 </file>
@@ -960,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +991,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -1032,7 +1017,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -1058,7 +1043,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -1079,136 +1064,6 @@
         <v>13</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1216,14 +1071,9 @@
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{9C0ED566-105A-45EC-9F5D-2B6A80AAEA2E}"/>
     <hyperlink ref="H3" r:id="rId2" xr:uid="{F27EE9C2-93C6-423C-941B-51CA677BD50A}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{7A624254-902A-4BE8-8480-03FE3700F71D}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{E4566D7D-C01A-4070-964A-F739FF3040F7}"/>
-    <hyperlink ref="H7" r:id="rId5" xr:uid="{2C9B3C80-90B8-4EA0-8911-74CC6FACB353}"/>
-    <hyperlink ref="H6" r:id="rId6" xr:uid="{212C05B1-9588-4458-9F5D-631E006F219F}"/>
-    <hyperlink ref="H9" r:id="rId7" xr:uid="{003A6616-76AE-4861-B59E-F6FAFCC0E2D2}"/>
-    <hyperlink ref="H8" r:id="rId8" xr:uid="{B323A4EC-E114-46C5-9BF6-E05C4D309059}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{96D7BFC8-9B38-4D6F-B6D0-A9B013F3216A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more comments on new randomizer
</commit_message>
<xml_diff>
--- a/WinnerWinnerChickenDinner/iattend output.xlsx
+++ b/WinnerWinnerChickenDinner/iattend output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\source\repos\WinnerWinnerChickenDinner\WinnerWinnerChickenDinner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D9EF6F-24E4-484D-A965-78DD3327DFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766CBC83-BA81-46CC-A35B-95948583DC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7035" yWindow="3420" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ticket Information" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="67">
   <si>
     <t>Number of tickets purchased</t>
   </si>
@@ -81,7 +81,157 @@
     <t>Edgar, Man</t>
   </si>
   <si>
-    <t>BEST WINNER</t>
+    <t>Asspol</t>
+  </si>
+  <si>
+    <t>Porral, Part</t>
+  </si>
+  <si>
+    <t>Bart Simpson</t>
+  </si>
+  <si>
+    <t>Yami, Dami</t>
+  </si>
+  <si>
+    <t>Just A Man</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>ssss</t>
+  </si>
+  <si>
+    <t>dddd</t>
+  </si>
+  <si>
+    <t>rrrrr</t>
+  </si>
+  <si>
+    <t>rrrrqq</t>
+  </si>
+  <si>
+    <t>wwqwe</t>
+  </si>
+  <si>
+    <t>qweasda</t>
+  </si>
+  <si>
+    <t>eqweqweq</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>zxcvzx</t>
+  </si>
+  <si>
+    <t>zxcvzxcv</t>
+  </si>
+  <si>
+    <t>reeeee</t>
+  </si>
+  <si>
+    <t>qweqwe</t>
+  </si>
+  <si>
+    <t>gjhjg</t>
+  </si>
+  <si>
+    <t>yuiyuiyu</t>
+  </si>
+  <si>
+    <t>iiuuuu</t>
+  </si>
+  <si>
+    <t>tyyyy</t>
+  </si>
+  <si>
+    <t>uyooppp</t>
+  </si>
+  <si>
+    <t>reeeeee</t>
+  </si>
+  <si>
+    <t>rtyyyy</t>
+  </si>
+  <si>
+    <t>uuuuu</t>
+  </si>
+  <si>
+    <t>yyyy</t>
+  </si>
+  <si>
+    <t>etrytryrt.</t>
+  </si>
+  <si>
+    <t>rtyrtyrty</t>
+  </si>
+  <si>
+    <t>ertyert</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>asddfdfffffff</t>
+  </si>
+  <si>
+    <t>zzzzzzsdss</t>
+  </si>
+  <si>
+    <t>serewr</t>
+  </si>
+  <si>
+    <t>rrreeeeeeeeeeee</t>
+  </si>
+  <si>
+    <t>ytuyuyuyuyurrr</t>
+  </si>
+  <si>
+    <t>tyuioooiiiiiuuu</t>
+  </si>
+  <si>
+    <t>yutytyfghfg</t>
+  </si>
+  <si>
+    <t>wertyeryeryery</t>
+  </si>
+  <si>
+    <t>sdfsdfsddfsd</t>
+  </si>
+  <si>
+    <t>hfghfghfghfgh</t>
+  </si>
+  <si>
+    <t>qwerqwerwer</t>
+  </si>
+  <si>
+    <t>sdfgsdfgtr</t>
+  </si>
+  <si>
+    <t>uytutyujijgh</t>
+  </si>
+  <si>
+    <t>tyuityutyuityu</t>
+  </si>
+  <si>
+    <t>ityuituityu</t>
+  </si>
+  <si>
+    <t>tyutyutyutyuty</t>
+  </si>
+  <si>
+    <t>eryertywetwetwe</t>
+  </si>
+  <si>
+    <t>utryuruy</t>
+  </si>
+  <si>
+    <t>eryeryeryer</t>
+  </si>
+  <si>
+    <t>wetwetwetwe</t>
   </si>
 </sst>
 </file>
@@ -945,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +1141,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -1017,7 +1167,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -1043,7 +1193,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -1064,6 +1214,1384 @@
         <v>13</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>10</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>10</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>10</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>10</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>10</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>10</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>10</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>10</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>10</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>10</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>10</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>10</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>10</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>10</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>10</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>10</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>10</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>10</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>10</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>10</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>10</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>10</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>10</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>10</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>10</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>10</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>10</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>10</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>10</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>10</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>10</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>10</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>10</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>10</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>10</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>10</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>10</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1071,9 +2599,62 @@
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{9C0ED566-105A-45EC-9F5D-2B6A80AAEA2E}"/>
     <hyperlink ref="H3" r:id="rId2" xr:uid="{F27EE9C2-93C6-423C-941B-51CA677BD50A}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{96D7BFC8-9B38-4D6F-B6D0-A9B013F3216A}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{7A624254-902A-4BE8-8480-03FE3700F71D}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{E4566D7D-C01A-4070-964A-F739FF3040F7}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{2C9B3C80-90B8-4EA0-8911-74CC6FACB353}"/>
+    <hyperlink ref="H6" r:id="rId6" xr:uid="{212C05B1-9588-4458-9F5D-631E006F219F}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{003A6616-76AE-4861-B59E-F6FAFCC0E2D2}"/>
+    <hyperlink ref="H8" r:id="rId8" xr:uid="{B323A4EC-E114-46C5-9BF6-E05C4D309059}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{10A8032D-E435-40F4-96A3-B1F93B0C23B8}"/>
+    <hyperlink ref="H11" r:id="rId10" xr:uid="{3B0BC544-A009-4EBF-92BB-035D67F2FAAE}"/>
+    <hyperlink ref="H12" r:id="rId11" xr:uid="{F3DD8712-727A-4CBD-8891-2EABC6C2BBB3}"/>
+    <hyperlink ref="H13" r:id="rId12" xr:uid="{DBF2D3FA-39C0-4F70-AD2D-868F300AD9FF}"/>
+    <hyperlink ref="H15" r:id="rId13" xr:uid="{BF0C57B8-0F43-4FD4-8AF4-9E562E3F01AF}"/>
+    <hyperlink ref="H14" r:id="rId14" xr:uid="{1AFEF47B-650E-4062-BF89-9E1567833457}"/>
+    <hyperlink ref="H17" r:id="rId15" xr:uid="{B85732E7-4641-492E-BE61-EBE7E37DA359}"/>
+    <hyperlink ref="H16" r:id="rId16" xr:uid="{DE5391A6-1FE3-4A55-A0DF-895DD785E58C}"/>
+    <hyperlink ref="H18" r:id="rId17" xr:uid="{C7A9E0C8-027A-48B1-BA51-B474BFF24A0B}"/>
+    <hyperlink ref="H19" r:id="rId18" xr:uid="{DEF7BB6F-F6AE-46E4-BC20-EF6B5C400BD9}"/>
+    <hyperlink ref="H20" r:id="rId19" xr:uid="{E6E33C10-01DB-4C5F-9680-145BC638655D}"/>
+    <hyperlink ref="H21" r:id="rId20" xr:uid="{D25646F9-B09C-4C96-8BF6-AE69A649BCC0}"/>
+    <hyperlink ref="H23" r:id="rId21" xr:uid="{215A4AF4-DD26-40BC-A3C4-1F25A28EC8FF}"/>
+    <hyperlink ref="H22" r:id="rId22" xr:uid="{B216B9AE-6824-40B3-86EB-70E3784F0E9F}"/>
+    <hyperlink ref="H25" r:id="rId23" xr:uid="{87224CF1-7438-4484-A061-C5FC68D792D3}"/>
+    <hyperlink ref="H24" r:id="rId24" xr:uid="{D655FC84-79C3-4B11-B00D-7D5390321A60}"/>
+    <hyperlink ref="H26" r:id="rId25" xr:uid="{0A4D12F9-C527-4AA5-8D19-98F9314DDB5E}"/>
+    <hyperlink ref="H27" r:id="rId26" xr:uid="{B35C7C62-DB26-40A1-AC1B-CB5EFD104C3D}"/>
+    <hyperlink ref="H28" r:id="rId27" xr:uid="{D7865154-C3AE-452A-9435-D89D24110FC0}"/>
+    <hyperlink ref="H29" r:id="rId28" xr:uid="{6816355D-7772-43A7-8E9C-FFA44484FB09}"/>
+    <hyperlink ref="H31" r:id="rId29" xr:uid="{63E38766-C914-4515-A34C-C8838CC45C72}"/>
+    <hyperlink ref="H30" r:id="rId30" xr:uid="{B9172E67-8073-4F45-86C2-0652B690E27E}"/>
+    <hyperlink ref="H33" r:id="rId31" xr:uid="{471F8CF4-5F62-41C4-9C6F-C95FB49097AA}"/>
+    <hyperlink ref="H32" r:id="rId32" xr:uid="{B1D2BBAA-D1C6-4112-828C-B17232D7E7E2}"/>
+    <hyperlink ref="H34" r:id="rId33" xr:uid="{0D55CF7C-2FDA-463F-A880-4A579634B8F9}"/>
+    <hyperlink ref="H35" r:id="rId34" xr:uid="{526A4020-629B-4FB8-845D-161DF309F02A}"/>
+    <hyperlink ref="H36" r:id="rId35" xr:uid="{2305F373-1AE7-447F-9BD6-1A1B51F58598}"/>
+    <hyperlink ref="H37" r:id="rId36" xr:uid="{65947F87-0488-4381-B766-7BC3C1E865C8}"/>
+    <hyperlink ref="H39" r:id="rId37" xr:uid="{1F046CA6-693F-4203-8A5F-1B4C3DC3041F}"/>
+    <hyperlink ref="H38" r:id="rId38" xr:uid="{52BB3586-4958-497E-A16D-6146158E0FDE}"/>
+    <hyperlink ref="H41" r:id="rId39" xr:uid="{018F945B-F6D0-4744-830B-FF4515C82631}"/>
+    <hyperlink ref="H40" r:id="rId40" xr:uid="{760DAE8D-22FD-462D-95E0-B3FDB745C911}"/>
+    <hyperlink ref="H42" r:id="rId41" xr:uid="{09450CF3-CABF-4E14-9464-733BDAE9751A}"/>
+    <hyperlink ref="H43" r:id="rId42" xr:uid="{BA4C1278-FD2E-48E9-9B23-8837A249B324}"/>
+    <hyperlink ref="H44" r:id="rId43" xr:uid="{1839BA6F-183C-470C-8166-47089781CB25}"/>
+    <hyperlink ref="H45" r:id="rId44" xr:uid="{C5077030-6EBF-42EF-A9E1-05E1AA09C03E}"/>
+    <hyperlink ref="H47" r:id="rId45" xr:uid="{1F03A538-2C92-4A6E-9BFA-2BEEA702EB05}"/>
+    <hyperlink ref="H46" r:id="rId46" xr:uid="{03261BBF-B78D-44E8-B4CC-04C1E436C27F}"/>
+    <hyperlink ref="H49" r:id="rId47" xr:uid="{457B1F2A-9873-4E21-8142-256C129DE235}"/>
+    <hyperlink ref="H48" r:id="rId48" xr:uid="{94993FC3-00B3-48EB-9575-0F86689AF671}"/>
+    <hyperlink ref="H50" r:id="rId49" xr:uid="{310F5F5B-0914-4586-9905-14FE8C4CA214}"/>
+    <hyperlink ref="H51" r:id="rId50" xr:uid="{8538BA83-C46B-447E-931C-1BC62A885249}"/>
+    <hyperlink ref="H52" r:id="rId51" xr:uid="{280114D4-962B-4F4B-B9BE-EFE718188C97}"/>
+    <hyperlink ref="H53" r:id="rId52" xr:uid="{4FDA95B3-84B2-484A-A5F1-57F1DBB1C016}"/>
+    <hyperlink ref="H55" r:id="rId53" xr:uid="{891D8B10-557A-47FC-AA02-DAD9C02E1F24}"/>
+    <hyperlink ref="H54" r:id="rId54" xr:uid="{1EC1A4C5-43EA-4177-843A-A1C7957A09D9}"/>
+    <hyperlink ref="H57" r:id="rId55" xr:uid="{264E7FBC-3A40-4ABF-BCBC-0DB6719A3486}"/>
+    <hyperlink ref="H56" r:id="rId56" xr:uid="{95B662C3-5822-4784-A6F6-FE7EB89C83DD}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
excel import changes, try catch for certain values, added multiple winner option into ticketlist.cs
</commit_message>
<xml_diff>
--- a/WinnerWinnerChickenDinner/iattend output.xlsx
+++ b/WinnerWinnerChickenDinner/iattend output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\source\repos\WinnerWinnerChickenDinner\WinnerWinnerChickenDinner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766CBC83-BA81-46CC-A35B-95948583DC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD539AEE-5372-4821-A596-AE3FDE2B643A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ticket Information" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="67">
   <si>
     <t>Number of tickets purchased</t>
   </si>
@@ -1097,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,9 +1184,7 @@
       <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="G3" s="4"/>
       <c r="H3" s="5" t="s">
         <v>14</v>
       </c>

</xml_diff>